<commit_message>
Completed preliminary test program
created a test program that reads cell voltages out to serial (raw adc
values, not scaled voltages). this sketch also contains a lot of
partially working functions for future functionality.

also updated was the atmega328 based master board. - which is not quite
complete
</commit_message>
<xml_diff>
--- a/Docs/OSBMS Slave BOM.xlsx
+++ b/Docs/OSBMS Slave BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Mouser #</t>
   </si>
@@ -51,9 +51,6 @@
     <t>CONN HEADER GH SIDE 9POS 1.25MM</t>
   </si>
   <si>
-    <t>spi bus connector</t>
-  </si>
-  <si>
     <t>455-1599-ND</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>CONN HEADER XH SIDE 7POS 2.5MM</t>
   </si>
   <si>
-    <t>battery connection header. may move to a dual pth/smd capable board</t>
-  </si>
-  <si>
     <t>455-2269-ND</t>
   </si>
   <si>
@@ -117,15 +111,6 @@
     <t>led resistor. leave out if not populating leds</t>
   </si>
   <si>
-    <t>279-352110RFT</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 3521 10R 1% 2W</t>
-  </si>
-  <si>
-    <t>will probably be replaced in the future with multiple smaller resistor packages</t>
-  </si>
-  <si>
     <t>859-LTST-C191KRKT</t>
   </si>
   <si>
@@ -150,27 +135,18 @@
     <t>Tantalum Capacitors - Solid SMD 6.3volts 33uF 3.2x1.6</t>
   </si>
   <si>
-    <t>min voltage 3.3v</t>
-  </si>
-  <si>
     <t>81-GRM188R61E105KA12</t>
   </si>
   <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 1uF 25volts X5R 10%</t>
   </si>
   <si>
-    <t>min voltage 5v</t>
-  </si>
-  <si>
     <t>963-GMK316F106ZL-T</t>
   </si>
   <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT Y5V 1206 35V 10uF +80/-20%</t>
   </si>
   <si>
-    <t>min voltage 30v - could possibly go for a larger vltage if 35v causes problems. (fully charged 6s lipo pack = 25.2v)</t>
-  </si>
-  <si>
     <t>9-10 pin ribbon cable</t>
   </si>
   <si>
@@ -205,6 +181,27 @@
   </si>
   <si>
     <t>~$1</t>
+  </si>
+  <si>
+    <t>4 needed per channel. Together they equal approximately 20 ohms</t>
+  </si>
+  <si>
+    <t>RNCP1206FTD82R5CT-ND</t>
+  </si>
+  <si>
+    <t>RES 82.5 OHM 1/2W 1% 1206</t>
+  </si>
+  <si>
+    <t>774-742C083102JP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor Networks &amp; Arrays 1Kohms 50V 5% </t>
+  </si>
+  <si>
+    <t>I love this thing. It cuts down the part count so much and makes everything much more compact.</t>
+  </si>
+  <si>
+    <t>battery connection header. Compatable with hobbyking battery 6s balance connectors. This may change</t>
   </si>
 </sst>
 </file>
@@ -584,385 +581,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" customWidth="1"/>
-    <col min="7" max="7" width="125.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="125.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="8">
+      <c r="G2" s="8">
         <v>6.9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2">
+      <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="9">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="9">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3">
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2">
+        <v>18</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="9">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2">
-        <v>18</v>
-      </c>
-      <c r="H5" s="9">
-        <v>1.89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="G10" s="9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="9">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="G11" s="9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="H7" s="9">
+      <c r="F12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2">
+        <v>24</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="9">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="9">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2">
-        <v>7</v>
-      </c>
-      <c r="H8" s="9">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="2">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="9">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="9">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="2">
         <v>2</v>
       </c>
-      <c r="H9" s="9">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2">
-        <v>6</v>
-      </c>
-      <c r="H10" s="9">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="9">
+      <c r="G25" s="6">
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2">
-        <v>6</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="9">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="2">
-        <v>6</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="9">
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="2">
-        <v>6</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="2">
-        <v>6</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="9">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="2">
-        <v>8</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="9">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="9">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="2" t="s">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" s="6">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="H23" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="2">
-        <v>2</v>
-      </c>
-      <c r="H24" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H26" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H27" s="6">
-        <f>SUM(H2:H18) +H23+H21+H24</f>
-        <v>18.5</v>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G28" s="6">
+        <f>SUM(G2:G19) +G24+G22+G25</f>
+        <v>17.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>